<commit_message>
Particle filtering for two parameters
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -406,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -444,8 +444,8 @@
         <v>34000</v>
       </c>
       <c r="C2" s="2">
-        <f>B2*0.66</f>
-        <v>22440</v>
+        <f>E2/2</f>
+        <v>224400</v>
       </c>
       <c r="D2" s="2">
         <v>578000</v>
@@ -463,8 +463,8 @@
         <v>70000</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ref="C3:C66" si="0">B3*0.66</f>
-        <v>46200</v>
+        <f t="shared" ref="C3:C66" si="0">E3/2</f>
+        <v>924000</v>
       </c>
       <c r="D3" s="2">
         <v>233333.33333333334</v>
@@ -483,7 +483,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" si="0"/>
-        <v>30360</v>
+        <v>288420</v>
       </c>
       <c r="D4" s="2">
         <v>141066.66666666669</v>
@@ -502,7 +502,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" si="0"/>
-        <v>7920</v>
+        <v>10560</v>
       </c>
       <c r="D5" s="2">
         <v>13090.90909090909</v>
@@ -521,7 +521,7 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" si="0"/>
-        <v>33000</v>
+        <v>511500</v>
       </c>
       <c r="D6" s="2">
         <v>80645.161290322576</v>
@@ -540,7 +540,7 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" si="0"/>
-        <v>37620</v>
+        <v>310365</v>
       </c>
       <c r="D7" s="2">
         <v>270750</v>
@@ -559,7 +559,7 @@
       </c>
       <c r="C8" s="2">
         <f t="shared" si="0"/>
-        <v>48180</v>
+        <v>240900</v>
       </c>
       <c r="D8" s="2">
         <v>111020.83333333333</v>
@@ -578,7 +578,7 @@
       </c>
       <c r="C9" s="2">
         <f t="shared" si="0"/>
-        <v>11220</v>
+        <v>5610</v>
       </c>
       <c r="D9" s="2">
         <v>12041.666666666668</v>
@@ -597,7 +597,7 @@
       </c>
       <c r="C10" s="2">
         <f t="shared" si="0"/>
-        <v>15840</v>
+        <v>26400</v>
       </c>
       <c r="D10" s="2">
         <v>44307.692307692312</v>
@@ -616,7 +616,7 @@
       </c>
       <c r="C11" s="2">
         <f t="shared" si="0"/>
-        <v>19800</v>
+        <v>8100.0000000000009</v>
       </c>
       <c r="D11" s="2">
         <v>16981.132075471698</v>
@@ -635,7 +635,7 @@
       </c>
       <c r="C12" s="2">
         <f t="shared" si="0"/>
-        <v>32340</v>
+        <v>759990</v>
       </c>
       <c r="D12" s="2">
         <v>160066.66666666666</v>
@@ -654,7 +654,7 @@
       </c>
       <c r="C13" s="2">
         <f t="shared" si="0"/>
-        <v>35640</v>
+        <v>356400</v>
       </c>
       <c r="D13" s="2">
         <v>72900</v>
@@ -673,7 +673,7 @@
       </c>
       <c r="C14" s="2">
         <f t="shared" si="0"/>
-        <v>22440</v>
+        <v>224400</v>
       </c>
       <c r="D14" s="2">
         <v>578000</v>
@@ -692,7 +692,7 @@
       </c>
       <c r="C15" s="2">
         <f t="shared" si="0"/>
-        <v>46200</v>
+        <v>924000</v>
       </c>
       <c r="D15" s="2">
         <v>233333.33333333334</v>
@@ -711,7 +711,7 @@
       </c>
       <c r="C16" s="2">
         <f t="shared" si="0"/>
-        <v>30360</v>
+        <v>288420</v>
       </c>
       <c r="D16" s="2">
         <v>141066.66666666669</v>
@@ -730,7 +730,7 @@
       </c>
       <c r="C17" s="2">
         <f t="shared" si="0"/>
-        <v>7920</v>
+        <v>10560</v>
       </c>
       <c r="D17" s="2">
         <v>13090.90909090909</v>
@@ -749,7 +749,7 @@
       </c>
       <c r="C18" s="2">
         <f t="shared" si="0"/>
-        <v>33000</v>
+        <v>511500</v>
       </c>
       <c r="D18" s="2">
         <v>80645.161290322576</v>
@@ -768,7 +768,7 @@
       </c>
       <c r="C19" s="2">
         <f t="shared" si="0"/>
-        <v>37620</v>
+        <v>310365</v>
       </c>
       <c r="D19" s="2">
         <v>270750</v>
@@ -787,7 +787,7 @@
       </c>
       <c r="C20" s="2">
         <f t="shared" si="0"/>
-        <v>48180</v>
+        <v>240900</v>
       </c>
       <c r="D20" s="2">
         <v>111020.83333333333</v>
@@ -806,7 +806,7 @@
       </c>
       <c r="C21" s="2">
         <f t="shared" si="0"/>
-        <v>11220</v>
+        <v>5610</v>
       </c>
       <c r="D21" s="2">
         <v>12041.666666666668</v>
@@ -825,7 +825,7 @@
       </c>
       <c r="C22" s="2">
         <f t="shared" si="0"/>
-        <v>15840</v>
+        <v>26400</v>
       </c>
       <c r="D22" s="2">
         <v>44307.692307692312</v>
@@ -844,7 +844,7 @@
       </c>
       <c r="C23" s="2">
         <f t="shared" si="0"/>
-        <v>19800</v>
+        <v>8100.0000000000009</v>
       </c>
       <c r="D23" s="2">
         <v>16981.132075471698</v>
@@ -863,7 +863,7 @@
       </c>
       <c r="C24" s="2">
         <f t="shared" si="0"/>
-        <v>32340</v>
+        <v>759990</v>
       </c>
       <c r="D24" s="2">
         <v>160066.66666666666</v>
@@ -882,7 +882,7 @@
       </c>
       <c r="C25" s="2">
         <f t="shared" si="0"/>
-        <v>35640</v>
+        <v>356400</v>
       </c>
       <c r="D25" s="2">
         <v>72900</v>
@@ -901,7 +901,7 @@
       </c>
       <c r="C26" s="2">
         <f t="shared" si="0"/>
-        <v>22440</v>
+        <v>224400</v>
       </c>
       <c r="D26" s="2">
         <v>578000</v>
@@ -920,7 +920,7 @@
       </c>
       <c r="C27" s="2">
         <f t="shared" si="0"/>
-        <v>46200</v>
+        <v>924000</v>
       </c>
       <c r="D27" s="2">
         <v>233333.33333333334</v>
@@ -939,7 +939,7 @@
       </c>
       <c r="C28" s="2">
         <f t="shared" si="0"/>
-        <v>30360</v>
+        <v>288420</v>
       </c>
       <c r="D28" s="2">
         <v>141066.66666666669</v>
@@ -958,7 +958,7 @@
       </c>
       <c r="C29" s="2">
         <f t="shared" si="0"/>
-        <v>7920</v>
+        <v>10560</v>
       </c>
       <c r="D29" s="2">
         <v>13090.90909090909</v>
@@ -977,7 +977,7 @@
       </c>
       <c r="C30" s="2">
         <f t="shared" si="0"/>
-        <v>33000</v>
+        <v>511500</v>
       </c>
       <c r="D30" s="2">
         <v>80645.161290322576</v>
@@ -996,7 +996,7 @@
       </c>
       <c r="C31" s="2">
         <f t="shared" si="0"/>
-        <v>37620</v>
+        <v>310365</v>
       </c>
       <c r="D31" s="2">
         <v>270750</v>
@@ -1015,7 +1015,7 @@
       </c>
       <c r="C32" s="2">
         <f t="shared" si="0"/>
-        <v>48180</v>
+        <v>240900</v>
       </c>
       <c r="D32" s="2">
         <v>111020.83333333333</v>
@@ -1034,7 +1034,7 @@
       </c>
       <c r="C33" s="2">
         <f t="shared" si="0"/>
-        <v>11220</v>
+        <v>5610</v>
       </c>
       <c r="D33" s="2">
         <v>12041.666666666668</v>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="C34" s="2">
         <f t="shared" si="0"/>
-        <v>15840</v>
+        <v>26400</v>
       </c>
       <c r="D34" s="2">
         <v>44307.692307692312</v>
@@ -1072,7 +1072,7 @@
       </c>
       <c r="C35" s="2">
         <f t="shared" si="0"/>
-        <v>19800</v>
+        <v>8100.0000000000009</v>
       </c>
       <c r="D35" s="2">
         <v>16981.132075471698</v>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="C36" s="2">
         <f t="shared" si="0"/>
-        <v>32340</v>
+        <v>759990</v>
       </c>
       <c r="D36" s="2">
         <v>160066.66666666666</v>
@@ -1110,7 +1110,7 @@
       </c>
       <c r="C37" s="2">
         <f t="shared" si="0"/>
-        <v>35640</v>
+        <v>356400</v>
       </c>
       <c r="D37" s="2">
         <v>72900</v>
@@ -1129,7 +1129,7 @@
       </c>
       <c r="C38" s="2">
         <f t="shared" si="0"/>
-        <v>22440</v>
+        <v>224400</v>
       </c>
       <c r="D38" s="2">
         <v>578000</v>
@@ -1148,7 +1148,7 @@
       </c>
       <c r="C39" s="2">
         <f t="shared" si="0"/>
-        <v>46200</v>
+        <v>924000</v>
       </c>
       <c r="D39" s="2">
         <v>233333.33333333334</v>
@@ -1167,7 +1167,7 @@
       </c>
       <c r="C40" s="2">
         <f t="shared" si="0"/>
-        <v>30360</v>
+        <v>288420</v>
       </c>
       <c r="D40" s="2">
         <v>141066.66666666669</v>
@@ -1186,7 +1186,7 @@
       </c>
       <c r="C41" s="2">
         <f t="shared" si="0"/>
-        <v>7920</v>
+        <v>10560</v>
       </c>
       <c r="D41" s="2">
         <v>13090.90909090909</v>
@@ -1205,7 +1205,7 @@
       </c>
       <c r="C42" s="2">
         <f t="shared" si="0"/>
-        <v>33000</v>
+        <v>511500</v>
       </c>
       <c r="D42" s="2">
         <v>80645.161290322576</v>
@@ -1224,7 +1224,7 @@
       </c>
       <c r="C43" s="2">
         <f t="shared" si="0"/>
-        <v>37620</v>
+        <v>310365</v>
       </c>
       <c r="D43" s="2">
         <v>270750</v>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="C44" s="2">
         <f t="shared" si="0"/>
-        <v>48180</v>
+        <v>240900</v>
       </c>
       <c r="D44" s="2">
         <v>111020.83333333333</v>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="C45" s="2">
         <f t="shared" si="0"/>
-        <v>11220</v>
+        <v>5610</v>
       </c>
       <c r="D45" s="2">
         <v>12041.666666666668</v>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="C46" s="2">
         <f t="shared" si="0"/>
-        <v>15840</v>
+        <v>26400</v>
       </c>
       <c r="D46" s="2">
         <v>44307.692307692312</v>
@@ -1300,7 +1300,7 @@
       </c>
       <c r="C47" s="2">
         <f t="shared" si="0"/>
-        <v>19800</v>
+        <v>8100.0000000000009</v>
       </c>
       <c r="D47" s="2">
         <v>16981.132075471698</v>
@@ -1319,7 +1319,7 @@
       </c>
       <c r="C48" s="2">
         <f t="shared" si="0"/>
-        <v>32340</v>
+        <v>759990</v>
       </c>
       <c r="D48" s="2">
         <v>160066.66666666666</v>
@@ -1338,7 +1338,7 @@
       </c>
       <c r="C49" s="2">
         <f t="shared" si="0"/>
-        <v>35640</v>
+        <v>356400</v>
       </c>
       <c r="D49" s="2">
         <v>72900</v>
@@ -1357,7 +1357,7 @@
       </c>
       <c r="C50" s="2">
         <f t="shared" si="0"/>
-        <v>22440</v>
+        <v>224400</v>
       </c>
       <c r="D50" s="2">
         <v>578000</v>
@@ -1376,7 +1376,7 @@
       </c>
       <c r="C51" s="2">
         <f t="shared" si="0"/>
-        <v>46200</v>
+        <v>924000</v>
       </c>
       <c r="D51" s="2">
         <v>233333.33333333334</v>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="C52" s="2">
         <f t="shared" si="0"/>
-        <v>30360</v>
+        <v>288420</v>
       </c>
       <c r="D52" s="2">
         <v>141066.66666666669</v>
@@ -1414,7 +1414,7 @@
       </c>
       <c r="C53" s="2">
         <f t="shared" si="0"/>
-        <v>7920</v>
+        <v>10560</v>
       </c>
       <c r="D53" s="2">
         <v>13090.90909090909</v>
@@ -1433,7 +1433,7 @@
       </c>
       <c r="C54" s="2">
         <f t="shared" si="0"/>
-        <v>33000</v>
+        <v>511500</v>
       </c>
       <c r="D54" s="2">
         <v>80645.161290322576</v>
@@ -1452,7 +1452,7 @@
       </c>
       <c r="C55" s="2">
         <f t="shared" si="0"/>
-        <v>37620</v>
+        <v>310365</v>
       </c>
       <c r="D55" s="2">
         <v>270750</v>
@@ -1471,7 +1471,7 @@
       </c>
       <c r="C56" s="2">
         <f t="shared" si="0"/>
-        <v>48180</v>
+        <v>240900</v>
       </c>
       <c r="D56" s="2">
         <v>111020.83333333333</v>
@@ -1490,7 +1490,7 @@
       </c>
       <c r="C57" s="2">
         <f t="shared" si="0"/>
-        <v>11220</v>
+        <v>5610</v>
       </c>
       <c r="D57" s="2">
         <v>12041.666666666668</v>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="C58" s="2">
         <f t="shared" si="0"/>
-        <v>15840</v>
+        <v>26400</v>
       </c>
       <c r="D58" s="2">
         <v>44307.692307692312</v>
@@ -1528,7 +1528,7 @@
       </c>
       <c r="C59" s="2">
         <f t="shared" si="0"/>
-        <v>19800</v>
+        <v>8100.0000000000009</v>
       </c>
       <c r="D59" s="2">
         <v>16981.132075471698</v>
@@ -1547,7 +1547,7 @@
       </c>
       <c r="C60" s="2">
         <f t="shared" si="0"/>
-        <v>32340</v>
+        <v>759990</v>
       </c>
       <c r="D60" s="2">
         <v>160066.66666666666</v>
@@ -1566,7 +1566,7 @@
       </c>
       <c r="C61" s="2">
         <f t="shared" si="0"/>
-        <v>35640</v>
+        <v>356400</v>
       </c>
       <c r="D61" s="2">
         <v>72900</v>
@@ -1585,7 +1585,7 @@
       </c>
       <c r="C62" s="2">
         <f t="shared" si="0"/>
-        <v>22440</v>
+        <v>224400</v>
       </c>
       <c r="D62" s="2">
         <v>578000</v>
@@ -1604,7 +1604,7 @@
       </c>
       <c r="C63" s="2">
         <f t="shared" si="0"/>
-        <v>46200</v>
+        <v>924000</v>
       </c>
       <c r="D63" s="2">
         <v>233333.33333333334</v>
@@ -1623,7 +1623,7 @@
       </c>
       <c r="C64" s="2">
         <f t="shared" si="0"/>
-        <v>30360</v>
+        <v>288420</v>
       </c>
       <c r="D64" s="2">
         <v>141066.66666666669</v>
@@ -1642,7 +1642,7 @@
       </c>
       <c r="C65" s="2">
         <f t="shared" si="0"/>
-        <v>7920</v>
+        <v>10560</v>
       </c>
       <c r="D65" s="2">
         <v>13090.90909090909</v>
@@ -1661,7 +1661,7 @@
       </c>
       <c r="C66" s="2">
         <f t="shared" si="0"/>
-        <v>33000</v>
+        <v>511500</v>
       </c>
       <c r="D66" s="2">
         <v>80645.161290322576</v>
@@ -1679,8 +1679,8 @@
         <v>57000</v>
       </c>
       <c r="C67" s="2">
-        <f t="shared" ref="C67:C85" si="2">B67*0.66</f>
-        <v>37620</v>
+        <f t="shared" ref="C67:C85" si="2">E67/2</f>
+        <v>310365</v>
       </c>
       <c r="D67" s="2">
         <v>270750</v>
@@ -1691,7 +1691,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <f t="shared" ref="A68:A85" si="3">A67+100</f>
+        <f t="shared" ref="A68:A131" si="3">A67+100</f>
         <v>6601</v>
       </c>
       <c r="B68" s="3">
@@ -1699,7 +1699,7 @@
       </c>
       <c r="C68" s="2">
         <f t="shared" si="2"/>
-        <v>48180</v>
+        <v>240900</v>
       </c>
       <c r="D68" s="2">
         <v>111020.83333333333</v>
@@ -1718,7 +1718,7 @@
       </c>
       <c r="C69" s="2">
         <f t="shared" si="2"/>
-        <v>11220</v>
+        <v>5610</v>
       </c>
       <c r="D69" s="2">
         <v>12041.666666666668</v>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="C70" s="2">
         <f t="shared" si="2"/>
-        <v>15840</v>
+        <v>26400</v>
       </c>
       <c r="D70" s="2">
         <v>44307.692307692312</v>
@@ -1756,7 +1756,7 @@
       </c>
       <c r="C71" s="2">
         <f t="shared" si="2"/>
-        <v>19800</v>
+        <v>8100.0000000000009</v>
       </c>
       <c r="D71" s="2">
         <v>16981.132075471698</v>
@@ -1775,7 +1775,7 @@
       </c>
       <c r="C72" s="2">
         <f t="shared" si="2"/>
-        <v>32340</v>
+        <v>759990</v>
       </c>
       <c r="D72" s="2">
         <v>160066.66666666666</v>
@@ -1794,7 +1794,7 @@
       </c>
       <c r="C73" s="2">
         <f t="shared" si="2"/>
-        <v>35640</v>
+        <v>356400</v>
       </c>
       <c r="D73" s="2">
         <v>72900</v>
@@ -1813,7 +1813,7 @@
       </c>
       <c r="C74" s="2">
         <f t="shared" si="2"/>
-        <v>22440</v>
+        <v>224400</v>
       </c>
       <c r="D74" s="2">
         <v>578000</v>
@@ -1832,7 +1832,7 @@
       </c>
       <c r="C75" s="2">
         <f t="shared" si="2"/>
-        <v>46200</v>
+        <v>924000</v>
       </c>
       <c r="D75" s="2">
         <v>233333.33333333334</v>
@@ -1851,7 +1851,7 @@
       </c>
       <c r="C76" s="2">
         <f t="shared" si="2"/>
-        <v>30360</v>
+        <v>288420</v>
       </c>
       <c r="D76" s="2">
         <v>141066.66666666669</v>
@@ -1870,7 +1870,7 @@
       </c>
       <c r="C77" s="2">
         <f t="shared" si="2"/>
-        <v>7920</v>
+        <v>10560</v>
       </c>
       <c r="D77" s="2">
         <v>13090.90909090909</v>
@@ -1889,7 +1889,7 @@
       </c>
       <c r="C78" s="2">
         <f t="shared" si="2"/>
-        <v>33000</v>
+        <v>511500</v>
       </c>
       <c r="D78" s="2">
         <v>80645.161290322576</v>
@@ -1908,7 +1908,7 @@
       </c>
       <c r="C79" s="2">
         <f t="shared" si="2"/>
-        <v>37620</v>
+        <v>310365</v>
       </c>
       <c r="D79" s="2">
         <v>270750</v>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="C80" s="2">
         <f t="shared" si="2"/>
-        <v>48180</v>
+        <v>240900</v>
       </c>
       <c r="D80" s="2">
         <v>111020.83333333333</v>
@@ -1946,7 +1946,7 @@
       </c>
       <c r="C81" s="2">
         <f t="shared" si="2"/>
-        <v>11220</v>
+        <v>5610</v>
       </c>
       <c r="D81" s="2">
         <v>12041.666666666668</v>
@@ -1965,7 +1965,7 @@
       </c>
       <c r="C82" s="2">
         <f t="shared" si="2"/>
-        <v>15840</v>
+        <v>26400</v>
       </c>
       <c r="D82" s="2">
         <v>44307.692307692312</v>
@@ -1984,7 +1984,7 @@
       </c>
       <c r="C83" s="2">
         <f t="shared" si="2"/>
-        <v>19800</v>
+        <v>8100.0000000000009</v>
       </c>
       <c r="D83" s="2">
         <v>16981.132075471698</v>
@@ -2003,7 +2003,7 @@
       </c>
       <c r="C84" s="2">
         <f t="shared" si="2"/>
-        <v>32340</v>
+        <v>759990</v>
       </c>
       <c r="D84" s="2">
         <v>160066.66666666666</v>
@@ -2022,12 +2022,1608 @@
       </c>
       <c r="C85" s="2">
         <f t="shared" si="2"/>
-        <v>35640</v>
+        <v>356400</v>
       </c>
       <c r="D85" s="2">
         <v>72900</v>
       </c>
       <c r="E85" s="2">
+        <v>712800</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <f t="shared" si="3"/>
+        <v>8401</v>
+      </c>
+      <c r="B86" s="3">
+        <v>34000</v>
+      </c>
+      <c r="C86" s="2">
+        <f>E86/2</f>
+        <v>224400</v>
+      </c>
+      <c r="D86" s="2">
+        <v>578000</v>
+      </c>
+      <c r="E86" s="2">
+        <v>448800</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <f t="shared" si="3"/>
+        <v>8501</v>
+      </c>
+      <c r="B87" s="3">
+        <v>70000</v>
+      </c>
+      <c r="C87" s="2">
+        <f t="shared" ref="C87:C150" si="4">E87/2</f>
+        <v>924000</v>
+      </c>
+      <c r="D87" s="2">
+        <v>233333.33333333334</v>
+      </c>
+      <c r="E87" s="2">
+        <v>1848000</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <f t="shared" si="3"/>
+        <v>8601</v>
+      </c>
+      <c r="B88" s="3">
+        <v>46000</v>
+      </c>
+      <c r="C88" s="2">
+        <f t="shared" si="4"/>
+        <v>288420</v>
+      </c>
+      <c r="D88" s="2">
+        <v>141066.66666666669</v>
+      </c>
+      <c r="E88" s="2">
+        <v>576840</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <f t="shared" si="3"/>
+        <v>8701</v>
+      </c>
+      <c r="B89" s="3">
+        <v>12000</v>
+      </c>
+      <c r="C89" s="2">
+        <f t="shared" si="4"/>
+        <v>10560</v>
+      </c>
+      <c r="D89" s="2">
+        <v>13090.90909090909</v>
+      </c>
+      <c r="E89" s="2">
+        <v>21120</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <f t="shared" si="3"/>
+        <v>8801</v>
+      </c>
+      <c r="B90" s="3">
+        <v>50000</v>
+      </c>
+      <c r="C90" s="2">
+        <f t="shared" si="4"/>
+        <v>511500</v>
+      </c>
+      <c r="D90" s="2">
+        <v>80645.161290322576</v>
+      </c>
+      <c r="E90" s="2">
+        <v>1023000</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <f t="shared" si="3"/>
+        <v>8901</v>
+      </c>
+      <c r="B91" s="3">
+        <v>57000</v>
+      </c>
+      <c r="C91" s="2">
+        <f t="shared" si="4"/>
+        <v>310365</v>
+      </c>
+      <c r="D91" s="2">
+        <v>270750</v>
+      </c>
+      <c r="E91" s="2">
+        <v>620730</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <f t="shared" si="3"/>
+        <v>9001</v>
+      </c>
+      <c r="B92" s="3">
+        <v>73000</v>
+      </c>
+      <c r="C92" s="2">
+        <f t="shared" si="4"/>
+        <v>240900</v>
+      </c>
+      <c r="D92" s="2">
+        <v>111020.83333333333</v>
+      </c>
+      <c r="E92" s="2">
+        <v>481800</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <f t="shared" si="3"/>
+        <v>9101</v>
+      </c>
+      <c r="B93" s="3">
+        <v>17000</v>
+      </c>
+      <c r="C93" s="2">
+        <f t="shared" si="4"/>
+        <v>5610</v>
+      </c>
+      <c r="D93" s="2">
+        <v>12041.666666666668</v>
+      </c>
+      <c r="E93" s="2">
+        <v>11220</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <f t="shared" si="3"/>
+        <v>9201</v>
+      </c>
+      <c r="B94" s="3">
+        <v>24000</v>
+      </c>
+      <c r="C94" s="2">
+        <f t="shared" si="4"/>
+        <v>26400</v>
+      </c>
+      <c r="D94" s="2">
+        <v>44307.692307692312</v>
+      </c>
+      <c r="E94" s="2">
+        <v>52800</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <f t="shared" si="3"/>
+        <v>9301</v>
+      </c>
+      <c r="B95" s="3">
+        <v>30000</v>
+      </c>
+      <c r="C95" s="2">
+        <f t="shared" si="4"/>
+        <v>8100.0000000000009</v>
+      </c>
+      <c r="D95" s="2">
+        <v>16981.132075471698</v>
+      </c>
+      <c r="E95" s="2">
+        <v>16200.000000000002</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <f t="shared" si="3"/>
+        <v>9401</v>
+      </c>
+      <c r="B96" s="3">
+        <v>49000</v>
+      </c>
+      <c r="C96" s="2">
+        <f t="shared" si="4"/>
+        <v>759990</v>
+      </c>
+      <c r="D96" s="2">
+        <v>160066.66666666666</v>
+      </c>
+      <c r="E96" s="2">
+        <v>1519980</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <f t="shared" si="3"/>
+        <v>9501</v>
+      </c>
+      <c r="B97" s="3">
+        <v>54000</v>
+      </c>
+      <c r="C97" s="2">
+        <f t="shared" si="4"/>
+        <v>356400</v>
+      </c>
+      <c r="D97" s="2">
+        <v>72900</v>
+      </c>
+      <c r="E97" s="2">
+        <v>712800</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
+        <f t="shared" si="3"/>
+        <v>9601</v>
+      </c>
+      <c r="B98" s="3">
+        <v>34000</v>
+      </c>
+      <c r="C98" s="2">
+        <f t="shared" si="4"/>
+        <v>224400</v>
+      </c>
+      <c r="D98" s="2">
+        <v>578000</v>
+      </c>
+      <c r="E98" s="2">
+        <v>448800</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <f t="shared" si="3"/>
+        <v>9701</v>
+      </c>
+      <c r="B99" s="3">
+        <v>70000</v>
+      </c>
+      <c r="C99" s="2">
+        <f t="shared" si="4"/>
+        <v>924000</v>
+      </c>
+      <c r="D99" s="2">
+        <v>233333.33333333334</v>
+      </c>
+      <c r="E99" s="2">
+        <v>1848000</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <f t="shared" si="3"/>
+        <v>9801</v>
+      </c>
+      <c r="B100" s="3">
+        <v>46000</v>
+      </c>
+      <c r="C100" s="2">
+        <f t="shared" si="4"/>
+        <v>288420</v>
+      </c>
+      <c r="D100" s="2">
+        <v>141066.66666666669</v>
+      </c>
+      <c r="E100" s="2">
+        <v>576840</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <f t="shared" si="3"/>
+        <v>9901</v>
+      </c>
+      <c r="B101" s="3">
+        <v>12000</v>
+      </c>
+      <c r="C101" s="2">
+        <f t="shared" si="4"/>
+        <v>10560</v>
+      </c>
+      <c r="D101" s="2">
+        <v>13090.90909090909</v>
+      </c>
+      <c r="E101" s="2">
+        <v>21120</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <f t="shared" si="3"/>
+        <v>10001</v>
+      </c>
+      <c r="B102" s="3">
+        <v>50000</v>
+      </c>
+      <c r="C102" s="2">
+        <f t="shared" si="4"/>
+        <v>511500</v>
+      </c>
+      <c r="D102" s="2">
+        <v>80645.161290322576</v>
+      </c>
+      <c r="E102" s="2">
+        <v>1023000</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <f t="shared" si="3"/>
+        <v>10101</v>
+      </c>
+      <c r="B103" s="3">
+        <v>57000</v>
+      </c>
+      <c r="C103" s="2">
+        <f t="shared" si="4"/>
+        <v>310365</v>
+      </c>
+      <c r="D103" s="2">
+        <v>270750</v>
+      </c>
+      <c r="E103" s="2">
+        <v>620730</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="2">
+        <f t="shared" si="3"/>
+        <v>10201</v>
+      </c>
+      <c r="B104" s="3">
+        <v>73000</v>
+      </c>
+      <c r="C104" s="2">
+        <f t="shared" si="4"/>
+        <v>240900</v>
+      </c>
+      <c r="D104" s="2">
+        <v>111020.83333333333</v>
+      </c>
+      <c r="E104" s="2">
+        <v>481800</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="2">
+        <f t="shared" si="3"/>
+        <v>10301</v>
+      </c>
+      <c r="B105" s="3">
+        <v>17000</v>
+      </c>
+      <c r="C105" s="2">
+        <f t="shared" si="4"/>
+        <v>5610</v>
+      </c>
+      <c r="D105" s="2">
+        <v>12041.666666666668</v>
+      </c>
+      <c r="E105" s="2">
+        <v>11220</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="2">
+        <f t="shared" si="3"/>
+        <v>10401</v>
+      </c>
+      <c r="B106" s="3">
+        <v>24000</v>
+      </c>
+      <c r="C106" s="2">
+        <f t="shared" si="4"/>
+        <v>26400</v>
+      </c>
+      <c r="D106" s="2">
+        <v>44307.692307692312</v>
+      </c>
+      <c r="E106" s="2">
+        <v>52800</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="2">
+        <f t="shared" si="3"/>
+        <v>10501</v>
+      </c>
+      <c r="B107" s="3">
+        <v>30000</v>
+      </c>
+      <c r="C107" s="2">
+        <f t="shared" si="4"/>
+        <v>8100.0000000000009</v>
+      </c>
+      <c r="D107" s="2">
+        <v>16981.132075471698</v>
+      </c>
+      <c r="E107" s="2">
+        <v>16200.000000000002</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="2">
+        <f t="shared" si="3"/>
+        <v>10601</v>
+      </c>
+      <c r="B108" s="3">
+        <v>49000</v>
+      </c>
+      <c r="C108" s="2">
+        <f t="shared" si="4"/>
+        <v>759990</v>
+      </c>
+      <c r="D108" s="2">
+        <v>160066.66666666666</v>
+      </c>
+      <c r="E108" s="2">
+        <v>1519980</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="2">
+        <f t="shared" si="3"/>
+        <v>10701</v>
+      </c>
+      <c r="B109" s="3">
+        <v>54000</v>
+      </c>
+      <c r="C109" s="2">
+        <f t="shared" si="4"/>
+        <v>356400</v>
+      </c>
+      <c r="D109" s="2">
+        <v>72900</v>
+      </c>
+      <c r="E109" s="2">
+        <v>712800</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="2">
+        <f t="shared" si="3"/>
+        <v>10801</v>
+      </c>
+      <c r="B110" s="3">
+        <v>34000</v>
+      </c>
+      <c r="C110" s="2">
+        <f t="shared" si="4"/>
+        <v>224400</v>
+      </c>
+      <c r="D110" s="2">
+        <v>578000</v>
+      </c>
+      <c r="E110" s="2">
+        <v>448800</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="2">
+        <f t="shared" si="3"/>
+        <v>10901</v>
+      </c>
+      <c r="B111" s="3">
+        <v>70000</v>
+      </c>
+      <c r="C111" s="2">
+        <f t="shared" si="4"/>
+        <v>924000</v>
+      </c>
+      <c r="D111" s="2">
+        <v>233333.33333333334</v>
+      </c>
+      <c r="E111" s="2">
+        <v>1848000</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="2">
+        <f t="shared" si="3"/>
+        <v>11001</v>
+      </c>
+      <c r="B112" s="3">
+        <v>46000</v>
+      </c>
+      <c r="C112" s="2">
+        <f t="shared" si="4"/>
+        <v>288420</v>
+      </c>
+      <c r="D112" s="2">
+        <v>141066.66666666669</v>
+      </c>
+      <c r="E112" s="2">
+        <v>576840</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="2">
+        <f t="shared" si="3"/>
+        <v>11101</v>
+      </c>
+      <c r="B113" s="3">
+        <v>12000</v>
+      </c>
+      <c r="C113" s="2">
+        <f t="shared" si="4"/>
+        <v>10560</v>
+      </c>
+      <c r="D113" s="2">
+        <v>13090.90909090909</v>
+      </c>
+      <c r="E113" s="2">
+        <v>21120</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="2">
+        <f t="shared" si="3"/>
+        <v>11201</v>
+      </c>
+      <c r="B114" s="3">
+        <v>50000</v>
+      </c>
+      <c r="C114" s="2">
+        <f t="shared" si="4"/>
+        <v>511500</v>
+      </c>
+      <c r="D114" s="2">
+        <v>80645.161290322576</v>
+      </c>
+      <c r="E114" s="2">
+        <v>1023000</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="2">
+        <f t="shared" si="3"/>
+        <v>11301</v>
+      </c>
+      <c r="B115" s="3">
+        <v>57000</v>
+      </c>
+      <c r="C115" s="2">
+        <f t="shared" si="4"/>
+        <v>310365</v>
+      </c>
+      <c r="D115" s="2">
+        <v>270750</v>
+      </c>
+      <c r="E115" s="2">
+        <v>620730</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="2">
+        <f t="shared" si="3"/>
+        <v>11401</v>
+      </c>
+      <c r="B116" s="3">
+        <v>73000</v>
+      </c>
+      <c r="C116" s="2">
+        <f t="shared" si="4"/>
+        <v>240900</v>
+      </c>
+      <c r="D116" s="2">
+        <v>111020.83333333333</v>
+      </c>
+      <c r="E116" s="2">
+        <v>481800</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="2">
+        <f t="shared" si="3"/>
+        <v>11501</v>
+      </c>
+      <c r="B117" s="3">
+        <v>17000</v>
+      </c>
+      <c r="C117" s="2">
+        <f t="shared" si="4"/>
+        <v>5610</v>
+      </c>
+      <c r="D117" s="2">
+        <v>12041.666666666668</v>
+      </c>
+      <c r="E117" s="2">
+        <v>11220</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="2">
+        <f t="shared" si="3"/>
+        <v>11601</v>
+      </c>
+      <c r="B118" s="3">
+        <v>24000</v>
+      </c>
+      <c r="C118" s="2">
+        <f t="shared" si="4"/>
+        <v>26400</v>
+      </c>
+      <c r="D118" s="2">
+        <v>44307.692307692312</v>
+      </c>
+      <c r="E118" s="2">
+        <v>52800</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="2">
+        <f t="shared" si="3"/>
+        <v>11701</v>
+      </c>
+      <c r="B119" s="3">
+        <v>30000</v>
+      </c>
+      <c r="C119" s="2">
+        <f t="shared" si="4"/>
+        <v>8100.0000000000009</v>
+      </c>
+      <c r="D119" s="2">
+        <v>16981.132075471698</v>
+      </c>
+      <c r="E119" s="2">
+        <v>16200.000000000002</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="2">
+        <f t="shared" si="3"/>
+        <v>11801</v>
+      </c>
+      <c r="B120" s="3">
+        <v>49000</v>
+      </c>
+      <c r="C120" s="2">
+        <f t="shared" si="4"/>
+        <v>759990</v>
+      </c>
+      <c r="D120" s="2">
+        <v>160066.66666666666</v>
+      </c>
+      <c r="E120" s="2">
+        <v>1519980</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="2">
+        <f t="shared" si="3"/>
+        <v>11901</v>
+      </c>
+      <c r="B121" s="3">
+        <v>54000</v>
+      </c>
+      <c r="C121" s="2">
+        <f t="shared" si="4"/>
+        <v>356400</v>
+      </c>
+      <c r="D121" s="2">
+        <v>72900</v>
+      </c>
+      <c r="E121" s="2">
+        <v>712800</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="2">
+        <f t="shared" si="3"/>
+        <v>12001</v>
+      </c>
+      <c r="B122" s="3">
+        <v>34000</v>
+      </c>
+      <c r="C122" s="2">
+        <f t="shared" si="4"/>
+        <v>224400</v>
+      </c>
+      <c r="D122" s="2">
+        <v>578000</v>
+      </c>
+      <c r="E122" s="2">
+        <v>448800</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="2">
+        <f t="shared" si="3"/>
+        <v>12101</v>
+      </c>
+      <c r="B123" s="3">
+        <v>70000</v>
+      </c>
+      <c r="C123" s="2">
+        <f t="shared" si="4"/>
+        <v>924000</v>
+      </c>
+      <c r="D123" s="2">
+        <v>233333.33333333334</v>
+      </c>
+      <c r="E123" s="2">
+        <v>1848000</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="2">
+        <f t="shared" si="3"/>
+        <v>12201</v>
+      </c>
+      <c r="B124" s="3">
+        <v>46000</v>
+      </c>
+      <c r="C124" s="2">
+        <f t="shared" si="4"/>
+        <v>288420</v>
+      </c>
+      <c r="D124" s="2">
+        <v>141066.66666666669</v>
+      </c>
+      <c r="E124" s="2">
+        <v>576840</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="2">
+        <f t="shared" si="3"/>
+        <v>12301</v>
+      </c>
+      <c r="B125" s="3">
+        <v>12000</v>
+      </c>
+      <c r="C125" s="2">
+        <f t="shared" si="4"/>
+        <v>10560</v>
+      </c>
+      <c r="D125" s="2">
+        <v>13090.90909090909</v>
+      </c>
+      <c r="E125" s="2">
+        <v>21120</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="2">
+        <f t="shared" si="3"/>
+        <v>12401</v>
+      </c>
+      <c r="B126" s="3">
+        <v>50000</v>
+      </c>
+      <c r="C126" s="2">
+        <f t="shared" si="4"/>
+        <v>511500</v>
+      </c>
+      <c r="D126" s="2">
+        <v>80645.161290322576</v>
+      </c>
+      <c r="E126" s="2">
+        <v>1023000</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="2">
+        <f t="shared" si="3"/>
+        <v>12501</v>
+      </c>
+      <c r="B127" s="3">
+        <v>57000</v>
+      </c>
+      <c r="C127" s="2">
+        <f t="shared" si="4"/>
+        <v>310365</v>
+      </c>
+      <c r="D127" s="2">
+        <v>270750</v>
+      </c>
+      <c r="E127" s="2">
+        <v>620730</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="2">
+        <f t="shared" si="3"/>
+        <v>12601</v>
+      </c>
+      <c r="B128" s="3">
+        <v>73000</v>
+      </c>
+      <c r="C128" s="2">
+        <f t="shared" si="4"/>
+        <v>240900</v>
+      </c>
+      <c r="D128" s="2">
+        <v>111020.83333333333</v>
+      </c>
+      <c r="E128" s="2">
+        <v>481800</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="2">
+        <f t="shared" si="3"/>
+        <v>12701</v>
+      </c>
+      <c r="B129" s="3">
+        <v>17000</v>
+      </c>
+      <c r="C129" s="2">
+        <f t="shared" si="4"/>
+        <v>5610</v>
+      </c>
+      <c r="D129" s="2">
+        <v>12041.666666666668</v>
+      </c>
+      <c r="E129" s="2">
+        <v>11220</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="2">
+        <f t="shared" si="3"/>
+        <v>12801</v>
+      </c>
+      <c r="B130" s="3">
+        <v>24000</v>
+      </c>
+      <c r="C130" s="2">
+        <f t="shared" si="4"/>
+        <v>26400</v>
+      </c>
+      <c r="D130" s="2">
+        <v>44307.692307692312</v>
+      </c>
+      <c r="E130" s="2">
+        <v>52800</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="2">
+        <f t="shared" si="3"/>
+        <v>12901</v>
+      </c>
+      <c r="B131" s="3">
+        <v>30000</v>
+      </c>
+      <c r="C131" s="2">
+        <f t="shared" si="4"/>
+        <v>8100.0000000000009</v>
+      </c>
+      <c r="D131" s="2">
+        <v>16981.132075471698</v>
+      </c>
+      <c r="E131" s="2">
+        <v>16200.000000000002</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="2">
+        <f t="shared" ref="A132:A169" si="5">A131+100</f>
+        <v>13001</v>
+      </c>
+      <c r="B132" s="3">
+        <v>49000</v>
+      </c>
+      <c r="C132" s="2">
+        <f t="shared" si="4"/>
+        <v>759990</v>
+      </c>
+      <c r="D132" s="2">
+        <v>160066.66666666666</v>
+      </c>
+      <c r="E132" s="2">
+        <v>1519980</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="2">
+        <f t="shared" si="5"/>
+        <v>13101</v>
+      </c>
+      <c r="B133" s="3">
+        <v>54000</v>
+      </c>
+      <c r="C133" s="2">
+        <f t="shared" si="4"/>
+        <v>356400</v>
+      </c>
+      <c r="D133" s="2">
+        <v>72900</v>
+      </c>
+      <c r="E133" s="2">
+        <v>712800</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="2">
+        <f t="shared" si="5"/>
+        <v>13201</v>
+      </c>
+      <c r="B134" s="3">
+        <v>34000</v>
+      </c>
+      <c r="C134" s="2">
+        <f t="shared" si="4"/>
+        <v>224400</v>
+      </c>
+      <c r="D134" s="2">
+        <v>578000</v>
+      </c>
+      <c r="E134" s="2">
+        <v>448800</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="2">
+        <f t="shared" si="5"/>
+        <v>13301</v>
+      </c>
+      <c r="B135" s="3">
+        <v>70000</v>
+      </c>
+      <c r="C135" s="2">
+        <f t="shared" si="4"/>
+        <v>924000</v>
+      </c>
+      <c r="D135" s="2">
+        <v>233333.33333333334</v>
+      </c>
+      <c r="E135" s="2">
+        <v>1848000</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="2">
+        <f t="shared" si="5"/>
+        <v>13401</v>
+      </c>
+      <c r="B136" s="3">
+        <v>46000</v>
+      </c>
+      <c r="C136" s="2">
+        <f t="shared" si="4"/>
+        <v>288420</v>
+      </c>
+      <c r="D136" s="2">
+        <v>141066.66666666669</v>
+      </c>
+      <c r="E136" s="2">
+        <v>576840</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="2">
+        <f t="shared" si="5"/>
+        <v>13501</v>
+      </c>
+      <c r="B137" s="3">
+        <v>12000</v>
+      </c>
+      <c r="C137" s="2">
+        <f t="shared" si="4"/>
+        <v>10560</v>
+      </c>
+      <c r="D137" s="2">
+        <v>13090.90909090909</v>
+      </c>
+      <c r="E137" s="2">
+        <v>21120</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="2">
+        <f t="shared" si="5"/>
+        <v>13601</v>
+      </c>
+      <c r="B138" s="3">
+        <v>50000</v>
+      </c>
+      <c r="C138" s="2">
+        <f t="shared" si="4"/>
+        <v>511500</v>
+      </c>
+      <c r="D138" s="2">
+        <v>80645.161290322576</v>
+      </c>
+      <c r="E138" s="2">
+        <v>1023000</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="2">
+        <f t="shared" si="5"/>
+        <v>13701</v>
+      </c>
+      <c r="B139" s="3">
+        <v>57000</v>
+      </c>
+      <c r="C139" s="2">
+        <f t="shared" si="4"/>
+        <v>310365</v>
+      </c>
+      <c r="D139" s="2">
+        <v>270750</v>
+      </c>
+      <c r="E139" s="2">
+        <v>620730</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="2">
+        <f t="shared" si="5"/>
+        <v>13801</v>
+      </c>
+      <c r="B140" s="3">
+        <v>73000</v>
+      </c>
+      <c r="C140" s="2">
+        <f t="shared" si="4"/>
+        <v>240900</v>
+      </c>
+      <c r="D140" s="2">
+        <v>111020.83333333333</v>
+      </c>
+      <c r="E140" s="2">
+        <v>481800</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="2">
+        <f t="shared" si="5"/>
+        <v>13901</v>
+      </c>
+      <c r="B141" s="3">
+        <v>17000</v>
+      </c>
+      <c r="C141" s="2">
+        <f t="shared" si="4"/>
+        <v>5610</v>
+      </c>
+      <c r="D141" s="2">
+        <v>12041.666666666668</v>
+      </c>
+      <c r="E141" s="2">
+        <v>11220</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="2">
+        <f t="shared" si="5"/>
+        <v>14001</v>
+      </c>
+      <c r="B142" s="3">
+        <v>24000</v>
+      </c>
+      <c r="C142" s="2">
+        <f t="shared" si="4"/>
+        <v>26400</v>
+      </c>
+      <c r="D142" s="2">
+        <v>44307.692307692312</v>
+      </c>
+      <c r="E142" s="2">
+        <v>52800</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="2">
+        <f t="shared" si="5"/>
+        <v>14101</v>
+      </c>
+      <c r="B143" s="3">
+        <v>30000</v>
+      </c>
+      <c r="C143" s="2">
+        <f t="shared" si="4"/>
+        <v>8100.0000000000009</v>
+      </c>
+      <c r="D143" s="2">
+        <v>16981.132075471698</v>
+      </c>
+      <c r="E143" s="2">
+        <v>16200.000000000002</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="2">
+        <f t="shared" si="5"/>
+        <v>14201</v>
+      </c>
+      <c r="B144" s="3">
+        <v>49000</v>
+      </c>
+      <c r="C144" s="2">
+        <f t="shared" si="4"/>
+        <v>759990</v>
+      </c>
+      <c r="D144" s="2">
+        <v>160066.66666666666</v>
+      </c>
+      <c r="E144" s="2">
+        <v>1519980</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="2">
+        <f t="shared" si="5"/>
+        <v>14301</v>
+      </c>
+      <c r="B145" s="3">
+        <v>54000</v>
+      </c>
+      <c r="C145" s="2">
+        <f t="shared" si="4"/>
+        <v>356400</v>
+      </c>
+      <c r="D145" s="2">
+        <v>72900</v>
+      </c>
+      <c r="E145" s="2">
+        <v>712800</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="2">
+        <f t="shared" si="5"/>
+        <v>14401</v>
+      </c>
+      <c r="B146" s="3">
+        <v>34000</v>
+      </c>
+      <c r="C146" s="2">
+        <f t="shared" si="4"/>
+        <v>224400</v>
+      </c>
+      <c r="D146" s="2">
+        <v>578000</v>
+      </c>
+      <c r="E146" s="2">
+        <v>448800</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" s="2">
+        <f t="shared" si="5"/>
+        <v>14501</v>
+      </c>
+      <c r="B147" s="3">
+        <v>70000</v>
+      </c>
+      <c r="C147" s="2">
+        <f t="shared" si="4"/>
+        <v>924000</v>
+      </c>
+      <c r="D147" s="2">
+        <v>233333.33333333334</v>
+      </c>
+      <c r="E147" s="2">
+        <v>1848000</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="2">
+        <f t="shared" si="5"/>
+        <v>14601</v>
+      </c>
+      <c r="B148" s="3">
+        <v>46000</v>
+      </c>
+      <c r="C148" s="2">
+        <f t="shared" si="4"/>
+        <v>288420</v>
+      </c>
+      <c r="D148" s="2">
+        <v>141066.66666666669</v>
+      </c>
+      <c r="E148" s="2">
+        <v>576840</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="2">
+        <f t="shared" si="5"/>
+        <v>14701</v>
+      </c>
+      <c r="B149" s="3">
+        <v>12000</v>
+      </c>
+      <c r="C149" s="2">
+        <f t="shared" si="4"/>
+        <v>10560</v>
+      </c>
+      <c r="D149" s="2">
+        <v>13090.90909090909</v>
+      </c>
+      <c r="E149" s="2">
+        <v>21120</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="2">
+        <f t="shared" si="5"/>
+        <v>14801</v>
+      </c>
+      <c r="B150" s="3">
+        <v>50000</v>
+      </c>
+      <c r="C150" s="2">
+        <f t="shared" si="4"/>
+        <v>511500</v>
+      </c>
+      <c r="D150" s="2">
+        <v>80645.161290322576</v>
+      </c>
+      <c r="E150" s="2">
+        <v>1023000</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="2">
+        <f t="shared" si="5"/>
+        <v>14901</v>
+      </c>
+      <c r="B151" s="3">
+        <v>57000</v>
+      </c>
+      <c r="C151" s="2">
+        <f t="shared" ref="C151:C169" si="6">E151/2</f>
+        <v>310365</v>
+      </c>
+      <c r="D151" s="2">
+        <v>270750</v>
+      </c>
+      <c r="E151" s="2">
+        <v>620730</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="2">
+        <f t="shared" si="5"/>
+        <v>15001</v>
+      </c>
+      <c r="B152" s="3">
+        <v>73000</v>
+      </c>
+      <c r="C152" s="2">
+        <f t="shared" si="6"/>
+        <v>240900</v>
+      </c>
+      <c r="D152" s="2">
+        <v>111020.83333333333</v>
+      </c>
+      <c r="E152" s="2">
+        <v>481800</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="2">
+        <f t="shared" si="5"/>
+        <v>15101</v>
+      </c>
+      <c r="B153" s="3">
+        <v>17000</v>
+      </c>
+      <c r="C153" s="2">
+        <f t="shared" si="6"/>
+        <v>5610</v>
+      </c>
+      <c r="D153" s="2">
+        <v>12041.666666666668</v>
+      </c>
+      <c r="E153" s="2">
+        <v>11220</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="2">
+        <f t="shared" si="5"/>
+        <v>15201</v>
+      </c>
+      <c r="B154" s="3">
+        <v>24000</v>
+      </c>
+      <c r="C154" s="2">
+        <f t="shared" si="6"/>
+        <v>26400</v>
+      </c>
+      <c r="D154" s="2">
+        <v>44307.692307692312</v>
+      </c>
+      <c r="E154" s="2">
+        <v>52800</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="2">
+        <f t="shared" si="5"/>
+        <v>15301</v>
+      </c>
+      <c r="B155" s="3">
+        <v>30000</v>
+      </c>
+      <c r="C155" s="2">
+        <f t="shared" si="6"/>
+        <v>8100.0000000000009</v>
+      </c>
+      <c r="D155" s="2">
+        <v>16981.132075471698</v>
+      </c>
+      <c r="E155" s="2">
+        <v>16200.000000000002</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="2">
+        <f t="shared" si="5"/>
+        <v>15401</v>
+      </c>
+      <c r="B156" s="3">
+        <v>49000</v>
+      </c>
+      <c r="C156" s="2">
+        <f t="shared" si="6"/>
+        <v>759990</v>
+      </c>
+      <c r="D156" s="2">
+        <v>160066.66666666666</v>
+      </c>
+      <c r="E156" s="2">
+        <v>1519980</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="2">
+        <f t="shared" si="5"/>
+        <v>15501</v>
+      </c>
+      <c r="B157" s="3">
+        <v>54000</v>
+      </c>
+      <c r="C157" s="2">
+        <f t="shared" si="6"/>
+        <v>356400</v>
+      </c>
+      <c r="D157" s="2">
+        <v>72900</v>
+      </c>
+      <c r="E157" s="2">
+        <v>712800</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="2">
+        <f t="shared" si="5"/>
+        <v>15601</v>
+      </c>
+      <c r="B158" s="3">
+        <v>34000</v>
+      </c>
+      <c r="C158" s="2">
+        <f t="shared" si="6"/>
+        <v>224400</v>
+      </c>
+      <c r="D158" s="2">
+        <v>578000</v>
+      </c>
+      <c r="E158" s="2">
+        <v>448800</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="2">
+        <f t="shared" si="5"/>
+        <v>15701</v>
+      </c>
+      <c r="B159" s="3">
+        <v>70000</v>
+      </c>
+      <c r="C159" s="2">
+        <f t="shared" si="6"/>
+        <v>924000</v>
+      </c>
+      <c r="D159" s="2">
+        <v>233333.33333333334</v>
+      </c>
+      <c r="E159" s="2">
+        <v>1848000</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="2">
+        <f t="shared" si="5"/>
+        <v>15801</v>
+      </c>
+      <c r="B160" s="3">
+        <v>46000</v>
+      </c>
+      <c r="C160" s="2">
+        <f t="shared" si="6"/>
+        <v>288420</v>
+      </c>
+      <c r="D160" s="2">
+        <v>141066.66666666669</v>
+      </c>
+      <c r="E160" s="2">
+        <v>576840</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="2">
+        <f t="shared" si="5"/>
+        <v>15901</v>
+      </c>
+      <c r="B161" s="3">
+        <v>12000</v>
+      </c>
+      <c r="C161" s="2">
+        <f t="shared" si="6"/>
+        <v>10560</v>
+      </c>
+      <c r="D161" s="2">
+        <v>13090.90909090909</v>
+      </c>
+      <c r="E161" s="2">
+        <v>21120</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="2">
+        <f t="shared" si="5"/>
+        <v>16001</v>
+      </c>
+      <c r="B162" s="3">
+        <v>50000</v>
+      </c>
+      <c r="C162" s="2">
+        <f t="shared" si="6"/>
+        <v>511500</v>
+      </c>
+      <c r="D162" s="2">
+        <v>80645.161290322576</v>
+      </c>
+      <c r="E162" s="2">
+        <v>1023000</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="2">
+        <f t="shared" si="5"/>
+        <v>16101</v>
+      </c>
+      <c r="B163" s="3">
+        <v>57000</v>
+      </c>
+      <c r="C163" s="2">
+        <f t="shared" si="6"/>
+        <v>310365</v>
+      </c>
+      <c r="D163" s="2">
+        <v>270750</v>
+      </c>
+      <c r="E163" s="2">
+        <v>620730</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="2">
+        <f t="shared" si="5"/>
+        <v>16201</v>
+      </c>
+      <c r="B164" s="3">
+        <v>73000</v>
+      </c>
+      <c r="C164" s="2">
+        <f t="shared" si="6"/>
+        <v>240900</v>
+      </c>
+      <c r="D164" s="2">
+        <v>111020.83333333333</v>
+      </c>
+      <c r="E164" s="2">
+        <v>481800</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="2">
+        <f t="shared" si="5"/>
+        <v>16301</v>
+      </c>
+      <c r="B165" s="3">
+        <v>17000</v>
+      </c>
+      <c r="C165" s="2">
+        <f t="shared" si="6"/>
+        <v>5610</v>
+      </c>
+      <c r="D165" s="2">
+        <v>12041.666666666668</v>
+      </c>
+      <c r="E165" s="2">
+        <v>11220</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="2">
+        <f t="shared" si="5"/>
+        <v>16401</v>
+      </c>
+      <c r="B166" s="3">
+        <v>24000</v>
+      </c>
+      <c r="C166" s="2">
+        <f t="shared" si="6"/>
+        <v>26400</v>
+      </c>
+      <c r="D166" s="2">
+        <v>44307.692307692312</v>
+      </c>
+      <c r="E166" s="2">
+        <v>52800</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="2">
+        <f t="shared" si="5"/>
+        <v>16501</v>
+      </c>
+      <c r="B167" s="3">
+        <v>30000</v>
+      </c>
+      <c r="C167" s="2">
+        <f t="shared" si="6"/>
+        <v>8100.0000000000009</v>
+      </c>
+      <c r="D167" s="2">
+        <v>16981.132075471698</v>
+      </c>
+      <c r="E167" s="2">
+        <v>16200.000000000002</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="2">
+        <f t="shared" si="5"/>
+        <v>16601</v>
+      </c>
+      <c r="B168" s="3">
+        <v>49000</v>
+      </c>
+      <c r="C168" s="2">
+        <f t="shared" si="6"/>
+        <v>759990</v>
+      </c>
+      <c r="D168" s="2">
+        <v>160066.66666666666</v>
+      </c>
+      <c r="E168" s="2">
+        <v>1519980</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="2">
+        <f t="shared" si="5"/>
+        <v>16701</v>
+      </c>
+      <c r="B169" s="3">
+        <v>54000</v>
+      </c>
+      <c r="C169" s="2">
+        <f t="shared" si="6"/>
+        <v>356400</v>
+      </c>
+      <c r="D169" s="2">
+        <v>72900</v>
+      </c>
+      <c r="E169" s="2">
         <v>712800</v>
       </c>
     </row>

</xml_diff>